<commit_message>
Initial work on SUT
</commit_message>
<xml_diff>
--- a/India Supply Use Table SUT_12-13_dated_280916_working_copy.xlsx
+++ b/India Supply Use Table SUT_12-13_dated_280916_working_copy.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="supply 2012-13" sheetId="1" r:id="rId1"/>
     <sheet name="Use 2012-13" sheetId="9" r:id="rId2"/>
+    <sheet name="Rates" sheetId="10" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'supply 2012-13'!$A$3:$CB$147</definedName>
@@ -25,7 +26,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'supply 2012-13'!$A:$B,'supply 2012-13'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Use 2012-13'!$A:$B,'Use 2012-13'!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="236">
   <si>
     <t>Value in Rs Lakh</t>
   </si>
@@ -801,6 +802,12 @@
   <si>
     <t>Supply Table 2012-13</t>
   </si>
+  <si>
+    <t>Product_ID</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
 </sst>
 </file>
 
@@ -811,7 +818,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -981,7 +988,7 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1019,10 +1026,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Comma" xfId="14" builtinId="3"/>
@@ -1343,12 +1351,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AC4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="BQ149" sqref="BQ149"/>
       <selection pane="topRight" activeCell="BQ149" sqref="BQ149"/>
       <selection pane="bottomLeft" activeCell="BQ149" sqref="BQ149"/>
-      <selection pane="bottomRight" activeCell="AI12" sqref="AI12"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55945,4 +55953,1156 @@
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B88" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A92" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B92" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B96" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B99" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A103" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B103" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B104" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B105" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B106" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B107" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B108" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B109" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B110" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B111" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B112" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B113" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A114" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B114" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B115" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B116" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B117" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B118" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="B119" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B120" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B121" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B122" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B123" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B124" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A125" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B125" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B126" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B127" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B128" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B129" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B130" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B131" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A132" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B132" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A133" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B133" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B134" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A135" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B135" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A136" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B136" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A137" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B137" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B138" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A139" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B139" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A140" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B140" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A141" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B141" s="19">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B142" s="19"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B143" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>